<commit_message>
Excel updated with column for test case reference
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="UserPermissions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>UserName</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>UserPermission</t>
   </si>
 </sst>
 </file>
@@ -363,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -371,41 +377,48 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed The Excel Format
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>TestCase</t>
   </si>
   <si>
     <t>UserPermission</t>
@@ -369,56 +366,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the format color
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -64,12 +64,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -84,8 +96,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -369,7 +383,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,18 +394,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Data Excel Updated.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/WebAutomationTestData.xlsx
+++ b/src/test/resources/testdata/WebAutomationTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>UserName</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>isAddButtonVisisble</t>
-  </si>
-  <si>
     <t>finance_read_only</t>
   </si>
   <si>
@@ -49,6 +46,12 @@
   </si>
   <si>
     <t>UserPermission</t>
+  </si>
+  <si>
+    <t>searchDocument_isEditable</t>
+  </si>
+  <si>
+    <t>missingClient_isEditable</t>
   </si>
 </sst>
 </file>
@@ -380,25 +383,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="28.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -406,29 +410,38 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>